<commit_message>
feat: added columns, flags and comp description
</commit_message>
<xml_diff>
--- a/public/scores.xlsx
+++ b/public/scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haraldstuge/Documents/NTNU-V24/Njord/ScoreBoard/my-csv-project-kopi/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomw\Documents\Njord\Competition2024\Scoreboard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2958678-101F-DD44-AC01-91E880A0EB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9920FEE6-AD1B-4351-9138-0886B9C4F21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{15966FE1-CA08-4D4D-8952-EF23C26B3292}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{15966FE1-CA08-4D4D-8952-EF23C26B3292}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Team Name</t>
   </si>
@@ -44,15 +44,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>AutoBee</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
     <t>Vortex</t>
   </si>
   <si>
@@ -65,19 +56,43 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>BagPiped</t>
-  </si>
-  <si>
     <t>Scotland</t>
   </si>
   <si>
-    <t>Vortex 2</t>
-  </si>
-  <si>
-    <t>Bag 2</t>
-  </si>
-  <si>
-    <t>Tallerone</t>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Total score</t>
+  </si>
+  <si>
+    <t>Day score</t>
+  </si>
+  <si>
+    <t>Time ranking</t>
+  </si>
+  <si>
+    <t>Running order</t>
+  </si>
+  <si>
+    <t>StrathVoyager</t>
+  </si>
+  <si>
+    <t>Navier USN</t>
+  </si>
+  <si>
+    <t>Team Aritra</t>
+  </si>
+  <si>
+    <t>AGH Solar Boat</t>
+  </si>
+  <si>
+    <t>Técnico Solar Boat</t>
   </si>
 </sst>
 </file>
@@ -449,15 +464,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2139CA8-6B11-924D-ADF5-3061163BEF6B}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,87 +484,160 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>95</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>99</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D5">
+        <v>98</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>95</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
+      <c r="D7">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>